<commit_message>
script edited from C
</commit_message>
<xml_diff>
--- a/data/casimport-correct.xlsx
+++ b/data/casimport-correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\git\pogoksci\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029CACE4-1A2E-4A67-8EDA-5EFE74DE55B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C943E285-D22B-4C5A-93F4-6D58AF1DC77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="330" windowWidth="22950" windowHeight="15480" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
+    <workbookView xWindow="3285" yWindow="0" windowWidth="22950" windowHeight="15480" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
   </bookViews>
   <sheets>
     <sheet name="casimport-correct" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t>녹말</t>
   </si>
   <si>
-    <t>(C&lt;sub&gt;6&lt;/sub&gt;H&lt;sub&gt;1&lt;/sub&gt;&lt;sub&gt;0&lt;/sub&gt;O&lt;sub&gt;5&lt;/sub&gt;)&lt;sub&gt;n(/sub&gt;</t>
-  </si>
-  <si>
     <t>"5743-47-5"</t>
   </si>
   <si>
@@ -584,10 +581,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>(C&lt;sub&gt;6&lt;/sub&gt;H&gt;sub&gt;7&lt;/sub&gt;O&lt;sub&gt;6&lt;/sub&gt;Na)&lt;sub&gt;n&lt;/sub&gt;</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>C&lt;sub&gt;25&lt;/sub&gt;H&lt;sub&gt;30&lt;/sub&gt;N&lt;sub&gt;3&lt;/sub&gt;·Cl</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -885,6 +878,14 @@
   </si>
   <si>
     <t>페로시안화 칼륨 3수화물</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(C&lt;sub&gt;6&lt;/sub&gt;H&lt;sub&gt;7&lt;/sub&gt;O&lt;sub&gt;6&lt;/sub&gt;Na)&lt;sub&gt;n&lt;/sub&gt;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(C&lt;sub&gt;6&lt;/sub&gt;H&lt;sub&gt;1&lt;/sub&gt;&lt;sub&gt;0&lt;/sub&gt;O&lt;sub&gt;5&lt;/sub&gt;)&lt;sub&gt;n&lt;/sub&gt;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1859,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D36CBED-76BA-4DBB-8B90-C0FC12620E70}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1881,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1895,40 +1896,40 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>201</v>
-      </c>
-      <c r="B2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" t="s">
         <v>235</v>
-      </c>
-      <c r="B4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1941,35 +1942,35 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" t="s">
         <v>238</v>
-      </c>
-      <c r="B7" t="s">
-        <v>239</v>
-      </c>
-      <c r="E7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" t="s">
         <v>204</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
         <v>186</v>
-      </c>
-      <c r="B9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1982,13 +1983,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -2013,7 +2014,7 @@
         <v>381.37</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -2043,21 +2044,21 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" t="s">
         <v>160</v>
-      </c>
-      <c r="E16" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
         <v>142</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>143</v>
-      </c>
-      <c r="E17" t="s">
-        <v>144</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2068,7 +2069,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C18">
         <v>231.54</v>
@@ -2079,38 +2080,38 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B19" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" t="s">
         <v>194</v>
-      </c>
-      <c r="B19" t="s">
-        <v>195</v>
-      </c>
-      <c r="E19" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="s">
         <v>162</v>
-      </c>
-      <c r="B20" t="s">
-        <v>163</v>
       </c>
       <c r="C20">
         <v>122.06</v>
       </c>
       <c r="E20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" t="s">
         <v>224</v>
-      </c>
-      <c r="B21" t="s">
-        <v>225</v>
-      </c>
-      <c r="E21" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2134,27 +2135,27 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B25" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C25">
         <v>422.39</v>
       </c>
       <c r="E25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2181,10 +2182,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2198,7 +2199,7 @@
         <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2206,7 +2207,7 @@
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
         <v>55</v>
@@ -2214,21 +2215,21 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" t="s">
         <v>132</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>133</v>
-      </c>
-      <c r="E31" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2253,71 +2254,71 @@
         <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" t="s">
         <v>126</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>127</v>
       </c>
-      <c r="D35" t="s">
-        <v>128</v>
-      </c>
       <c r="E35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" t="s">
         <v>138</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>139</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>140</v>
-      </c>
-      <c r="E36" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" t="s">
         <v>191</v>
-      </c>
-      <c r="B37" t="s">
-        <v>192</v>
-      </c>
-      <c r="D37" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" t="s">
         <v>129</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>130</v>
       </c>
-      <c r="D38" t="s">
-        <v>131</v>
-      </c>
       <c r="E38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" t="s">
         <v>172</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
         <v>173</v>
-      </c>
-      <c r="E39" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2331,18 +2332,18 @@
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" t="s">
         <v>149</v>
       </c>
-      <c r="B41" t="s">
-        <v>150</v>
-      </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2361,46 +2362,46 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" t="s">
+        <v>214</v>
+      </c>
+      <c r="E44" t="s">
         <v>215</v>
-      </c>
-      <c r="B44" t="s">
-        <v>216</v>
-      </c>
-      <c r="E44" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>195</v>
+      </c>
+      <c r="B46" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" t="s">
         <v>197</v>
-      </c>
-      <c r="B46" t="s">
-        <v>198</v>
-      </c>
-      <c r="E46" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2454,13 +2455,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>242</v>
+      </c>
+      <c r="B52" t="s">
+        <v>243</v>
+      </c>
+      <c r="E52" t="s">
         <v>244</v>
-      </c>
-      <c r="B52" t="s">
-        <v>245</v>
-      </c>
-      <c r="E52" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2476,13 +2477,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B54" t="s">
+        <v>230</v>
+      </c>
+      <c r="E54" t="s">
         <v>232</v>
-      </c>
-      <c r="E54" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2534,18 +2535,18 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" t="s">
         <v>147</v>
-      </c>
-      <c r="E60" t="s">
-        <v>148</v>
       </c>
       <c r="F60">
         <v>3</v>
@@ -2567,10 +2568,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="E62" t="s">
         <v>145</v>
-      </c>
-      <c r="E62" t="s">
-        <v>146</v>
       </c>
       <c r="F62">
         <v>2</v>
@@ -2633,13 +2634,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>239</v>
+      </c>
+      <c r="B68" t="s">
         <v>241</v>
       </c>
-      <c r="B68" t="s">
-        <v>243</v>
-      </c>
       <c r="E68" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2655,13 +2656,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" t="s">
         <v>164</v>
       </c>
-      <c r="B70" t="s">
+      <c r="E70" t="s">
         <v>165</v>
-      </c>
-      <c r="E70" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2677,13 +2678,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B72" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2721,13 +2722,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
+        <v>246</v>
+      </c>
+      <c r="E76" t="s">
         <v>247</v>
-      </c>
-      <c r="B76" t="s">
-        <v>248</v>
-      </c>
-      <c r="E76" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2735,7 +2736,7 @@
         <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E77" t="s">
         <v>106</v>
@@ -2752,7 +2753,7 @@
         <v>109</v>
       </c>
       <c r="E78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2768,24 +2769,24 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" t="s">
+        <v>208</v>
+      </c>
+      <c r="E80" t="s">
         <v>209</v>
-      </c>
-      <c r="B80" t="s">
-        <v>210</v>
-      </c>
-      <c r="E80" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>210</v>
+      </c>
+      <c r="B81" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" t="s">
         <v>212</v>
-      </c>
-      <c r="B81" t="s">
-        <v>213</v>
-      </c>
-      <c r="D81" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2807,34 +2808,34 @@
         <v>124</v>
       </c>
       <c r="E83" t="s">
-        <v>125</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>135</v>
+      </c>
+      <c r="B84" t="s">
         <v>136</v>
       </c>
-      <c r="B84" t="s">
-        <v>137</v>
-      </c>
       <c r="E84" t="s">
-        <v>177</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E85" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" t="s">
         <v>170</v>
-      </c>
-      <c r="B86" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script edited by A
</commit_message>
<xml_diff>
--- a/data/casimport-correct.xlsx
+++ b/data/casimport-correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\git\pogoksci\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0618267-7CE9-4C7E-9072-733763528CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B2E9FE-4732-47E9-B1F1-87DA785FC48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="0" windowWidth="22950" windowHeight="15480" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
+    <workbookView xWindow="912" yWindow="2328" windowWidth="38988" windowHeight="22716" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
   </bookViews>
   <sheets>
     <sheet name="casimport-correct" sheetId="1" r:id="rId1"/>
@@ -733,10 +733,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>CH3OCH3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>"521-31-3"</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -886,6 +882,10 @@
   </si>
   <si>
     <t>"9008-02-0"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH&lt;sub&gt;3&lt;/sub&gt;OCH&lt;sub&gt;3&lt;/sub&gt;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1860,21 +1860,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D36CBED-76BA-4DBB-8B90-C0FC12620E70}">
   <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.59765625" customWidth="1"/>
+    <col min="4" max="4" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="93.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>198</v>
       </c>
@@ -1905,26 +1905,26 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" t="s">
         <v>219</v>
       </c>
-      <c r="E3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" t="s">
         <v>232</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>233</v>
       </c>
-      <c r="E4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1940,18 +1940,18 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" t="s">
         <v>235</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>236</v>
       </c>
-      <c r="E7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>201</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>159</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>161</v>
       </c>
@@ -2100,21 +2100,21 @@
         <v>122.06</v>
       </c>
       <c r="E20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" t="s">
         <v>221</v>
       </c>
-      <c r="B21" t="s">
+      <c r="E21" t="s">
         <v>222</v>
       </c>
-      <c r="E21" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2133,23 +2133,23 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>134</v>
       </c>
       <c r="B24" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" t="s">
         <v>224</v>
       </c>
-      <c r="E24" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>167</v>
       </c>
       <c r="B25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C25">
         <v>422.39</v>
@@ -2158,7 +2158,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -2180,15 +2180,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" t="s">
         <v>226</v>
       </c>
-      <c r="E28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>131</v>
       </c>
@@ -2224,15 +2224,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>214</v>
+      </c>
+      <c r="B32" t="s">
         <v>215</v>
       </c>
-      <c r="B32" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>188</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>170</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -2382,10 +2382,10 @@
         <v>213</v>
       </c>
       <c r="E44" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>186</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>194</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>115</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>113</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>120</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>118</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>110</v>
       </c>
@@ -2453,18 +2453,18 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
+        <v>240</v>
+      </c>
+      <c r="B52" t="s">
         <v>241</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>242</v>
       </c>
-      <c r="E52" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -2475,18 +2475,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
+        <v>227</v>
+      </c>
+      <c r="B54" t="s">
         <v>228</v>
       </c>
-      <c r="B54" t="s">
-        <v>229</v>
-      </c>
       <c r="E54" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>44</v>
       </c>
@@ -2533,15 +2533,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
+        <v>216</v>
+      </c>
+      <c r="B59" t="s">
         <v>217</v>
       </c>
-      <c r="B59" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>146</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>144</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>96</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>99</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>32</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2632,18 +2632,18 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B68" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E68" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>90</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>93</v>
       </c>
@@ -2676,9 +2676,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B72" t="s">
         <v>182</v>
@@ -2687,7 +2687,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>87</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>102</v>
       </c>
@@ -2720,29 +2720,29 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
+        <v>243</v>
+      </c>
+      <c r="B76" t="s">
         <v>244</v>
       </c>
-      <c r="B76" t="s">
+      <c r="E76" t="s">
         <v>245</v>
       </c>
-      <c r="E76" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E77" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>206</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>209</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>123</v>
       </c>
@@ -2808,10 +2808,10 @@
         <v>124</v>
       </c>
       <c r="E83" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>135</v>
       </c>
@@ -2819,18 +2819,18 @@
         <v>136</v>
       </c>
       <c r="E84" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
script edited by B
</commit_message>
<xml_diff>
--- a/data/casimport-correct.xlsx
+++ b/data/casimport-correct.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud\git\pogoksci\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3610E062-D9F1-42A1-BE02-49466EF86662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF27777E-8569-454A-8DA8-37363417F604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="0" windowWidth="27510" windowHeight="15480" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
+    <workbookView xWindow="1155" yWindow="1110" windowWidth="21405" windowHeight="15300" xr2:uid="{E8EAD6B7-D095-4B7C-B3FF-3488144841BF}"/>
   </bookViews>
   <sheets>
     <sheet name="casimport-correct" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="275">
   <si>
     <t>cas_ref</t>
   </si>
@@ -480,9 +475,6 @@
     <t>"10025-77-1"</t>
   </si>
   <si>
-    <t>염화 제2철 6수화물</t>
-  </si>
-  <si>
     <t>FeCl&lt;sub&gt;3&lt;/sub&gt;·6H&lt;sub&gt;2&lt;/sub&gt;O</t>
   </si>
   <si>
@@ -522,9 +514,6 @@
     <t>"10125-13-0"</t>
   </si>
   <si>
-    <t>염화 제2구리 2수화물</t>
-  </si>
-  <si>
     <t>CuCl&lt;sub&gt;2&lt;/sub&gt;·2H&lt;sub&gt;2&lt;/sub&gt;O</t>
   </si>
   <si>
@@ -802,6 +791,78 @@
   </si>
   <si>
     <t>Potassium ferrocyanide trihydrate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"1317-38-0"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>산화 구리(II)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"1317-39-1"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>산화 구리(I)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cupper(II) oxide</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cupper(I) oxide</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"10025-70-4"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>염화 철(II) 6수화물</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>염화 구리(II) 2수화물</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>염화 스트론튬 6수화물</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"7447-41-8"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>염화 리튬</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LiCl</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SrCl&lt;sub&gt;2&lt;/sub&gt;·6H&lt;sub&gt;2&lt;/sub&gt;O</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"13463-67-7"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TiO&lt;sub&gt;2&lt;/sub&gt;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>"7487-88-9"</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MgSO&lt;sub&gt;4&lt;/sub&gt;</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1774,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D36CBED-76BA-4DBB-8B90-C0FC12620E70}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="B77" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1815,37 +1876,37 @@
         <v>150</v>
       </c>
       <c r="B2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" t="s">
         <v>151</v>
-      </c>
-      <c r="E2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" t="s">
         <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
         <v>155</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>156</v>
-      </c>
-      <c r="E4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1856,40 +1917,40 @@
         <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
         <v>161</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
         <v>162</v>
-      </c>
-      <c r="E7" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E8" t="s">
         <v>164</v>
-      </c>
-      <c r="B8" t="s">
-        <v>165</v>
-      </c>
-      <c r="E8" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" t="s">
         <v>167</v>
-      </c>
-      <c r="B9" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1902,13 +1963,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
         <v>170</v>
-      </c>
-      <c r="B11" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1933,10 +1994,10 @@
         <v>381.37</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1966,10 +2027,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1991,7 +2052,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C18">
         <v>231.54</v>
@@ -2002,10 +2063,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -2013,27 +2074,27 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C20">
         <v>122.06</v>
       </c>
       <c r="E20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" t="s">
         <v>183</v>
-      </c>
-      <c r="B21" t="s">
-        <v>184</v>
-      </c>
-      <c r="E21" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2060,27 +2121,27 @@
         <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C25">
         <v>422.39</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2107,10 +2168,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2124,7 +2185,7 @@
         <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2132,7 +2193,7 @@
         <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
         <v>55</v>
@@ -2151,10 +2212,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2179,7 +2240,7 @@
         <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2193,7 +2254,7 @@
         <v>127</v>
       </c>
       <c r="E35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2212,13 +2273,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" t="s">
         <v>199</v>
-      </c>
-      <c r="B37" t="s">
-        <v>200</v>
-      </c>
-      <c r="D37" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2229,21 +2290,21 @@
         <v>129</v>
       </c>
       <c r="D38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B39" t="s">
+        <v>203</v>
+      </c>
+      <c r="E39" t="s">
         <v>204</v>
-      </c>
-      <c r="B39" t="s">
-        <v>205</v>
-      </c>
-      <c r="E39" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2257,7 +2318,7 @@
         <v>40</v>
       </c>
       <c r="E40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2268,7 +2329,7 @@
         <v>148</v>
       </c>
       <c r="E41" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2287,49 +2348,49 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B43" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D43" t="s">
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" t="s">
         <v>212</v>
-      </c>
-      <c r="B44" t="s">
-        <v>213</v>
-      </c>
-      <c r="E44" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>215</v>
+      </c>
+      <c r="B46" t="s">
+        <v>216</v>
+      </c>
+      <c r="D46" t="s">
         <v>217</v>
       </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
         <v>218</v>
-      </c>
-      <c r="D46" t="s">
-        <v>219</v>
-      </c>
-      <c r="E46" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2383,13 +2444,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" t="s">
+        <v>220</v>
+      </c>
+      <c r="E52" t="s">
         <v>221</v>
-      </c>
-      <c r="B52" t="s">
-        <v>222</v>
-      </c>
-      <c r="E52" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -2405,13 +2466,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" t="s">
+        <v>223</v>
+      </c>
+      <c r="E54" t="s">
         <v>224</v>
-      </c>
-      <c r="B54" t="s">
-        <v>225</v>
-      </c>
-      <c r="E54" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2463,10 +2524,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B59" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -2546,7 +2607,7 @@
         <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E66" t="s">
         <v>17</v>
@@ -2565,13 +2626,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>228</v>
+      </c>
+      <c r="B68" t="s">
+        <v>229</v>
+      </c>
+      <c r="E68" t="s">
         <v>230</v>
-      </c>
-      <c r="B68" t="s">
-        <v>231</v>
-      </c>
-      <c r="E68" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -2587,13 +2648,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" t="s">
+        <v>232</v>
+      </c>
+      <c r="E70" t="s">
         <v>233</v>
-      </c>
-      <c r="B70" t="s">
-        <v>234</v>
-      </c>
-      <c r="E70" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -2609,13 +2670,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>234</v>
+      </c>
+      <c r="B72" t="s">
+        <v>235</v>
+      </c>
+      <c r="E72" t="s">
         <v>236</v>
-      </c>
-      <c r="B72" t="s">
-        <v>237</v>
-      </c>
-      <c r="E72" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -2653,13 +2714,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>237</v>
+      </c>
+      <c r="B76" t="s">
+        <v>238</v>
+      </c>
+      <c r="E76" t="s">
         <v>239</v>
-      </c>
-      <c r="B76" t="s">
-        <v>240</v>
-      </c>
-      <c r="E76" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -2667,7 +2728,7 @@
         <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E77" t="s">
         <v>106</v>
@@ -2684,7 +2745,7 @@
         <v>109</v>
       </c>
       <c r="E78" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -2700,24 +2761,24 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>242</v>
+      </c>
+      <c r="B80" t="s">
+        <v>243</v>
+      </c>
+      <c r="E80" t="s">
         <v>244</v>
-      </c>
-      <c r="B80" t="s">
-        <v>245</v>
-      </c>
-      <c r="E80" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>245</v>
+      </c>
+      <c r="B81" t="s">
+        <v>246</v>
+      </c>
+      <c r="D81" t="s">
         <v>247</v>
-      </c>
-      <c r="B81" t="s">
-        <v>248</v>
-      </c>
-      <c r="D81" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -2739,7 +2800,7 @@
         <v>124</v>
       </c>
       <c r="E83" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -2750,31 +2811,91 @@
         <v>135</v>
       </c>
       <c r="E84" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E86" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B87" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>257</v>
+      </c>
+      <c r="B88" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+      <c r="D89" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" t="s">
+        <v>266</v>
+      </c>
+      <c r="E90" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>267</v>
+      </c>
+      <c r="B91" t="s">
+        <v>268</v>
+      </c>
+      <c r="E91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>271</v>
+      </c>
+      <c r="E92" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>273</v>
+      </c>
+      <c r="E93" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -2783,5 +2904,6 @@
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>